<commit_message>
use dict_factory but not adaptable to None case
</commit_message>
<xml_diff>
--- a/output/risk_eval_output.xlsx
+++ b/output/risk_eval_output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12240" windowWidth="18915" xWindow="120" yWindow="135"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="120" yWindow="135" windowWidth="18915" windowHeight="12240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Risk Evaluation" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,23 +12,23 @@
     <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName hidden="1" name="_1_0Rwvu._Curren">[1]Sheet1!#REF!</definedName>
-    <definedName hidden="1" name="_2Rwvu._Curren">[1]Sheet1!#REF!</definedName>
-    <definedName hidden="1" name="ACwvu._Current_.">[1]Sheet1!#REF!</definedName>
-    <definedName hidden="1" name="crosstab_name">{"_10","Grand_total","_10","_6010","_10","_6015","_10","_6016","_80","_6018","_10","_20","_6020","_10","_6021","_10","_6031","_10","_6032","_10","_6034","_20","_6035","_10","_6040","_10","_6042","_10","_6060","_10","_20","_30","_6070","_10","_20","_6075","_10","_20","_30","_40","_6081","_10","_6111","_10","_20","_90","_6112","_10","_20","_6113","_10","_6120","_10","_6122","_10","_6131","_10","_6148","_10","_6153","_10","_6154","_10","_20","_40","_6161","_10","_6163","_10","_6170","_10","_6190","_10","_90","_6200","_10","_6211","_10","_6212","_10","_6213","_10","_6214","_10","_20","_6215","_10","_6216","_10","_6217","_10","_6218","_10","_20","_6220","_10","_20","_6225","_10","_20","_6226","_10","_30","_6227","_10","_20","_80","_6228","_10","_20","_30","_40","_6231","_10","_20","_30","_40","_6232","_10","_20","_30","_6234","_10","_6236","_90","_6239","_10","_20","_6261","_10","_20","_6265","_10","_20","_6267","_20","_30","_90","_6269","_10","_20","_30","_40","_50","_60","_70","_6290","_10","_20","_30","_60","_70","_6292","_90","_6299","_10","_6310","_10","_20","_90","_6311","_10","_20","_30","_6313","_10","_20","_30","_40","_50","_60","_70","_80","_90","_6315","_10","_6341","_20","_6391","_10","_6392","_10","_20","_6393","_90","_6399","_10","_20","_30","_6401","_10","_6412","_10","_6416","_10","_60","_70","_90","_6419","_10","_6421","_10","_6422","_10","_6423","_10","_6424","_10","_30","_90","_6429","_10","_20","_30","_6431","_10","_20","_6432","_10","_20","_30","_6441","_10","_6451","_10","_20","_30","_6471","_20","_6510","_10","_6520","_10","_30","_6597","_10","_40","_60","_70","_6598","_10","_20","_30","_40","_50","_80","_6599","_10","_6600","_10","_6601","_10","_6611","_10","_20","_30"}</definedName>
-    <definedName hidden="1" name="dd">{"resultado_resumen",#N/A,FALSE}</definedName>
-    <definedName hidden="1" name="dkfjs">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.completo.","ACwvu.resultado._.completo.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
-    <definedName hidden="1" name="eere">{"resultado completo",#N/A,FALSE}</definedName>
-    <definedName hidden="1" name="int_ext_sel">1</definedName>
-    <definedName hidden="1" name="Rwvu._Current_.">[1]Sheet1!#REF!</definedName>
-    <definedName hidden="1" name="sdfs">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.completo.","ACwvu.resultado._.completo.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
-    <definedName hidden="1" name="Swvu._Current_.">[1]Sheet1!#REF!</definedName>
-    <definedName hidden="1" name="wrn.resultado_resumen.">{"resultado_resumen",#N/A,FALSE}</definedName>
-    <definedName hidden="1" name="wrn.resultado_total.">{"resultado completo",#N/A,FALSE}</definedName>
-    <definedName hidden="1" name="wvu._Current_.">{TRUE,TRUE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,22,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu._Current_.","ACwvu._Current_.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7","Rwvu._Current_.",#N/A,FALSE,FALSE}</definedName>
-    <definedName hidden="1" name="wvu.resultado._.completo.">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.completo.","ACwvu.resultado._.completo.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
-    <definedName hidden="1" name="wvu.resultado._.resumen.">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.resumen.","ACwvu.resultado._.resumen.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
-    <definedName hidden="1" name="xxx">{"_10","Grand_total","_10","_6010","_10","_6015","_10","_6016","_80","_6018","_10","_20","_6020","_10","_6021","_10","_6031","_10","_6032","_10","_6034","_20","_6035","_10","_6040","_10","_6042","_10","_6060","_10","_20","_30","_6070","_10","_20","_6075","_10","_20","_30","_40","_6081","_10","_6111","_10","_20","_90","_6112","_10","_20","_6113","_10","_6120","_10","_6122","_10","_6131","_10","_6148","_10","_6153","_10","_6154","_10","_20","_40","_6161","_10","_6163","_10","_6170","_10","_6190","_10","_90","_6200","_10","_6211","_10","_6212","_10","_6213","_10","_6214","_10","_20","_6215","_10","_6216","_10","_6217","_10","_6218","_10","_20","_6220","_10","_20","_6225","_10","_20","_6226","_10","_30","_6227","_10","_20","_80","_6228","_10","_20","_30","_40","_6231","_10","_20","_30","_40","_6232","_10","_20","_30","_6234","_10","_6236","_90","_6239","_10","_20","_6261","_10","_20","_6265","_10","_20","_6267","_20","_30","_90","_6269","_10","_20","_30","_40","_50","_60","_70","_6290","_10","_20","_30","_60","_70","_6292","_90","_6299","_10","_6310","_10","_20","_90","_6311","_10","_20","_30","_6313","_10","_20","_30","_40","_50","_60","_70","_80","_90","_6315","_10","_6341","_20","_6391","_10","_6392","_10","_20","_6393","_90","_6399","_10","_20","_30","_6401","_10","_6412","_10","_6416","_10","_60","_70","_90","_6419","_10","_6421","_10","_6422","_10","_6423","_10","_6424","_10","_30","_90","_6429","_10","_20","_30","_6431","_10","_20","_6432","_10","_20","_30","_6441","_10","_6451","_10","_20","_30","_6471","_20","_6510","_10","_6520","_10","_30","_6597","_10","_40","_60","_70","_6598","_10","_20","_30","_40","_50","_80","_6599","_10","_6600","_10","_6601","_10","_6611","_10","_20","_30"}</definedName>
+    <definedName name="_1_0Rwvu._Curren" hidden="1">[1]Sheet1!#REF!</definedName>
+    <definedName name="_2Rwvu._Curren" hidden="1">[1]Sheet1!#REF!</definedName>
+    <definedName name="ACwvu._Current_." hidden="1">[1]Sheet1!#REF!</definedName>
+    <definedName name="crosstab_name" hidden="1">{"_10","Grand_total","_10","_6010","_10","_6015","_10","_6016","_80","_6018","_10","_20","_6020","_10","_6021","_10","_6031","_10","_6032","_10","_6034","_20","_6035","_10","_6040","_10","_6042","_10","_6060","_10","_20","_30","_6070","_10","_20","_6075","_10","_20","_30","_40","_6081","_10","_6111","_10","_20","_90","_6112","_10","_20","_6113","_10","_6120","_10","_6122","_10","_6131","_10","_6148","_10","_6153","_10","_6154","_10","_20","_40","_6161","_10","_6163","_10","_6170","_10","_6190","_10","_90","_6200","_10","_6211","_10","_6212","_10","_6213","_10","_6214","_10","_20","_6215","_10","_6216","_10","_6217","_10","_6218","_10","_20","_6220","_10","_20","_6225","_10","_20","_6226","_10","_30","_6227","_10","_20","_80","_6228","_10","_20","_30","_40","_6231","_10","_20","_30","_40","_6232","_10","_20","_30","_6234","_10","_6236","_90","_6239","_10","_20","_6261","_10","_20","_6265","_10","_20","_6267","_20","_30","_90","_6269","_10","_20","_30","_40","_50","_60","_70","_6290","_10","_20","_30","_60","_70","_6292","_90","_6299","_10","_6310","_10","_20","_90","_6311","_10","_20","_30","_6313","_10","_20","_30","_40","_50","_60","_70","_80","_90","_6315","_10","_6341","_20","_6391","_10","_6392","_10","_20","_6393","_90","_6399","_10","_20","_30","_6401","_10","_6412","_10","_6416","_10","_60","_70","_90","_6419","_10","_6421","_10","_6422","_10","_6423","_10","_6424","_10","_30","_90","_6429","_10","_20","_30","_6431","_10","_20","_6432","_10","_20","_30","_6441","_10","_6451","_10","_20","_30","_6471","_20","_6510","_10","_6520","_10","_30","_6597","_10","_40","_60","_70","_6598","_10","_20","_30","_40","_50","_80","_6599","_10","_6600","_10","_6601","_10","_6611","_10","_20","_30"}</definedName>
+    <definedName name="dd" hidden="1">{"resultado_resumen",#N/A,FALSE}</definedName>
+    <definedName name="dkfjs" hidden="1">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.completo.","ACwvu.resultado._.completo.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
+    <definedName name="eere" hidden="1">{"resultado completo",#N/A,FALSE}</definedName>
+    <definedName name="int_ext_sel" hidden="1">1</definedName>
+    <definedName name="Rwvu._Current_." hidden="1">[1]Sheet1!#REF!</definedName>
+    <definedName name="sdfs" hidden="1">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.completo.","ACwvu.resultado._.completo.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
+    <definedName name="Swvu._Current_." hidden="1">[1]Sheet1!#REF!</definedName>
+    <definedName name="wrn.resultado_resumen." hidden="1">{"resultado_resumen",#N/A,FALSE}</definedName>
+    <definedName name="wrn.resultado_total." hidden="1">{"resultado completo",#N/A,FALSE}</definedName>
+    <definedName name="wvu._Current_." hidden="1">{TRUE,TRUE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,22,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu._Current_.","ACwvu._Current_.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7","Rwvu._Current_.",#N/A,FALSE,FALSE}</definedName>
+    <definedName name="wvu.resultado._.completo." hidden="1">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.completo.","ACwvu.resultado._.completo.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
+    <definedName name="wvu.resultado._.resumen." hidden="1">{TRUE,FALSE,-2,-16.25,486,281.25,FALSE,FALSE,TRUE,TRUE,0,1,5,6,8,4,2,4,TRUE,TRUE,3,TRUE,1,TRUE,100,"Swvu.resultado._.resumen.","ACwvu.resultado._.resumen.",1,FALSE,FALSE,0.196850393700787,0.196850393700787,0.31496062992126,0.708661417322835,1,"","&amp;LAT AF/ Neumann&amp;CPage &amp;P&amp;R&amp;D   &amp;T   ",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R8C1:R460C22","=R1:R7",FALSE,FALSE,FALSE,FALSE}</definedName>
+    <definedName name="xxx" hidden="1">{"_10","Grand_total","_10","_6010","_10","_6015","_10","_6016","_80","_6018","_10","_20","_6020","_10","_6021","_10","_6031","_10","_6032","_10","_6034","_20","_6035","_10","_6040","_10","_6042","_10","_6060","_10","_20","_30","_6070","_10","_20","_6075","_10","_20","_30","_40","_6081","_10","_6111","_10","_20","_90","_6112","_10","_20","_6113","_10","_6120","_10","_6122","_10","_6131","_10","_6148","_10","_6153","_10","_6154","_10","_20","_40","_6161","_10","_6163","_10","_6170","_10","_6190","_10","_90","_6200","_10","_6211","_10","_6212","_10","_6213","_10","_6214","_10","_20","_6215","_10","_6216","_10","_6217","_10","_6218","_10","_20","_6220","_10","_20","_6225","_10","_20","_6226","_10","_30","_6227","_10","_20","_80","_6228","_10","_20","_30","_40","_6231","_10","_20","_30","_40","_6232","_10","_20","_30","_6234","_10","_6236","_90","_6239","_10","_20","_6261","_10","_20","_6265","_10","_20","_6267","_20","_30","_90","_6269","_10","_20","_30","_40","_50","_60","_70","_6290","_10","_20","_30","_60","_70","_6292","_90","_6299","_10","_6310","_10","_20","_90","_6311","_10","_20","_30","_6313","_10","_20","_30","_40","_50","_60","_70","_80","_90","_6315","_10","_6341","_20","_6391","_10","_6392","_10","_20","_6393","_90","_6399","_10","_20","_30","_6401","_10","_6412","_10","_6416","_10","_60","_70","_90","_6419","_10","_6421","_10","_6422","_10","_6423","_10","_6424","_10","_30","_90","_6429","_10","_20","_30","_6431","_10","_20","_6432","_10","_20","_30","_6441","_10","_6451","_10","_20","_30","_6471","_20","_6510","_10","_6520","_10","_30","_6597","_10","_40","_60","_70","_6598","_10","_20","_30","_40","_50","_80","_6599","_10","_6600","_10","_6601","_10","_6611","_10","_20","_30"}</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -37,10 +37,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt formatCode="#,##0.0" numFmtId="164"/>
-    <numFmt formatCode="&quot;N$&quot;#,##0_);[Red]\(&quot;N$&quot;#,##0\)" numFmtId="165"/>
-    <numFmt formatCode="&quot;N$&quot;#,##0.00_);[Red]\(&quot;N$&quot;#,##0.00\)" numFmtId="166"/>
-    <numFmt formatCode="_-* #,##0.00\ _P_t_s_-;\-* #,##0.00\ _P_t_s_-;_-* &quot;-&quot;??\ _P_t_s_-;_-@_-" numFmtId="167"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="&quot;N$&quot;#,##0_);[Red]\(&quot;N$&quot;#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="&quot;N$&quot;#,##0.00_);[Red]\(&quot;N$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _P_t_s_-;\-* #,##0.00\ _P_t_s_-;_-* &quot;-&quot;??\ _P_t_s_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1527,815 +1527,815 @@
     </border>
   </borders>
   <cellStyleXfs count="27">
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0"/>
-    <xf borderId="0" fillId="5" fontId="18" numFmtId="0"/>
-    <xf borderId="0" fillId="5" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="40" fontId="4" fillId="0" borderId="6"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="18" fillId="5" borderId="0"/>
+    <xf numFmtId="38" fontId="18" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="6" fontId="4" numFmtId="0">
-      <protection hidden="1" locked="1"/>
-    </xf>
-    <xf borderId="5" fillId="7" fontId="18" numFmtId="0"/>
-    <xf borderId="5" fillId="7" fontId="18" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="165"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="166"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="167"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyProtection="1">
+      <protection locked="1" hidden="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="7" borderId="5"/>
+    <xf numFmtId="10" fontId="18" fillId="7" borderId="5"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="40" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="266">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="27" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="28" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="29" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="30" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="31" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="32" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="33" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="34" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="7" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="41" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="42" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="43" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="44" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="23" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="22" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="23" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="45" fillId="4" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="46" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="27" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="28" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="29" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="30" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="31" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="29" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="29" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="52" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="54" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="54" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="52" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="55" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="56" fillId="4" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="57" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="57" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="58" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="36" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="29" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="36" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="49" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="49" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="50" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="50" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="52" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="31" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="60" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="61" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="61" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="62" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="63" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="60" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="61" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="61" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="62" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="63" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="56" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="64" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="65" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="65" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="57" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="57" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="32" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="33" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="34" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="48" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="50" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="67" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="37" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="50" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="67" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="74" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="74" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="75" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="75" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="76" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="76" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="77" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="77" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="78" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="78" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="59" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="54" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="70" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="71" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="70" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="71" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="22" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="24" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="53" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="35" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="23" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="24" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="48" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="30" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="52" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="29" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="52" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="31" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="29" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="30" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="31" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="34" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="35" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="54" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="41" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="36" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="36" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="29" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="57" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="58" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="56" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="58" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="33" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="27" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="28" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="48" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="32" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="48" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="35" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="68" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="69" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="65" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="68" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="69" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="66" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="27" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="28" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="64" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="66" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="26" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="26" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="36" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="12" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="12" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="19" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="46" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="47" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="4" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="13" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="13" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="14" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="25" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="26" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="19" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="19" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="72" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="72" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="73" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="73" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="13" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="23" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="23" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="38" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="40" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="39" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="74" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="75" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="51" fillId="8" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="43" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf borderId="76" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="77" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="78" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="54" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="71" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="86" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="84" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="88" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="25" fillId="2" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="79" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="82" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="83" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="23" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="89" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="91" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="53" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="24" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="94" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="96" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="61" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="39" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="99" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="62" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="19" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="96" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="21" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="95" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="60" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="44" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="97" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="98" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="98" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
     <cellStyle name="Befehl" xfId="2"/>
     <cellStyle name="Dezimal(0,0)" xfId="3"/>
@@ -2476,7 +2476,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -2495,9 +2495,9 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-      <sheetData refreshError="1" sheetId="3"/>
-      <sheetData refreshError="1" sheetId="4"/>
-      <sheetData refreshError="1" sheetId="5"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2830,21 +2830,21 @@
   </sheetPr>
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="25">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="25" workbookViewId="0">
       <selection activeCell="H7" sqref="H7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="2.7109375"/>
-    <col customWidth="1" max="2" min="2" width="15.140625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="8"/>
-    <col customWidth="1" max="4" min="4" width="24.140625"/>
-    <col customWidth="1" max="5" min="5" width="58.5703125"/>
-    <col customWidth="1" max="25" min="6" width="23"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="15.140625" customWidth="1" min="2" max="2"/>
+    <col width="8" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="24.140625" customWidth="1" min="4" max="4"/>
+    <col width="58.5703125" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="6" max="25"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="16.5" r="1">
+    <row r="1" ht="16.5" customHeight="1">
       <c r="A1" s="227" t="inlineStr">
         <is>
           <t>Risk Evaluation Components</t>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="E1" s="231" t="inlineStr">
         <is>
-          <t>GE APS GM Bev 3</t>
+          <t>APS VW MEB</t>
         </is>
       </c>
       <c r="F1" s="13" t="n"/>
@@ -2883,7 +2883,7 @@
       <c r="X1" s="13" t="n"/>
       <c r="Y1" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="2" thickBot="1">
+    <row r="2" ht="13.5" customHeight="1" thickBot="1">
       <c r="A2" s="232" t="n"/>
       <c r="B2" s="233" t="n"/>
       <c r="C2" s="234" t="n"/>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="Y3" s="238" t="n"/>
     </row>
-    <row customHeight="1" ht="32.25" r="4">
+    <row r="4" ht="32.25" customHeight="1">
       <c r="A4" s="209" t="inlineStr">
         <is>
           <t>Part Number
@@ -2983,21 +2983,33 @@
       <c r="E4" s="240" t="n"/>
       <c r="F4" s="213" t="inlineStr">
         <is>
-          <t>323.214-00</t>
+          <t>178.576-15</t>
         </is>
       </c>
       <c r="G4" s="241" t="n"/>
       <c r="H4" s="213" t="inlineStr">
         <is>
-          <t>323.215-00</t>
+          <t>191.674-01</t>
         </is>
       </c>
       <c r="I4" s="241" t="n"/>
-      <c r="J4" s="213" t="n"/>
+      <c r="J4" s="213" t="inlineStr">
+        <is>
+          <t>229.847-00</t>
+        </is>
+      </c>
       <c r="K4" s="241" t="n"/>
-      <c r="L4" s="213" t="n"/>
+      <c r="L4" s="213" t="inlineStr">
+        <is>
+          <t>234.536-00</t>
+        </is>
+      </c>
       <c r="M4" s="241" t="n"/>
-      <c r="N4" s="213" t="n"/>
+      <c r="N4" s="213" t="inlineStr">
+        <is>
+          <t>323.140-00</t>
+        </is>
+      </c>
       <c r="O4" s="241" t="n"/>
       <c r="P4" s="212" t="n"/>
       <c r="Q4" s="241" t="n"/>
@@ -3022,21 +3034,33 @@
       <c r="E5" s="240" t="n"/>
       <c r="F5" s="136" t="inlineStr">
         <is>
-          <t>BEDIENELEMENT</t>
+          <t>FEDER MONT-GR</t>
         </is>
       </c>
       <c r="G5" s="241" t="n"/>
       <c r="H5" s="136" t="inlineStr">
         <is>
-          <t>GEHAEUSE</t>
+          <t>STECKER GEHAEUSE MONT-GR</t>
         </is>
       </c>
       <c r="I5" s="241" t="n"/>
-      <c r="J5" s="136" t="n"/>
+      <c r="J5" s="136" t="inlineStr">
+        <is>
+          <t>BEDIENELEMENT</t>
+        </is>
+      </c>
       <c r="K5" s="241" t="n"/>
-      <c r="L5" s="136" t="n"/>
+      <c r="L5" s="136" t="inlineStr">
+        <is>
+          <t>GEHAEUSE MONT-GR</t>
+        </is>
+      </c>
       <c r="M5" s="241" t="n"/>
-      <c r="N5" s="136" t="n"/>
+      <c r="N5" s="136" t="inlineStr">
+        <is>
+          <t>GEHAEUSE MONT-GR</t>
+        </is>
+      </c>
       <c r="O5" s="241" t="n"/>
       <c r="P5" s="136" t="n"/>
       <c r="Q5" s="241" t="n"/>
@@ -3049,7 +3073,7 @@
       <c r="X5" s="136" t="n"/>
       <c r="Y5" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="12.75" outlineLevel="1" r="6">
+    <row r="6" outlineLevel="1" ht="12.75" customHeight="1">
       <c r="A6" s="209" t="inlineStr">
         <is>
           <t>Commodity Group</t>
@@ -3061,7 +3085,7 @@
       <c r="E6" s="240" t="n"/>
       <c r="F6" s="208" t="inlineStr">
         <is>
-          <t>TECH_PLAS</t>
+          <t>MET_EXTRU</t>
         </is>
       </c>
       <c r="G6" s="241" t="n"/>
@@ -3071,11 +3095,23 @@
         </is>
       </c>
       <c r="I6" s="241" t="n"/>
-      <c r="J6" s="208" t="n"/>
+      <c r="J6" s="208" t="inlineStr">
+        <is>
+          <t>TECH_PLAS</t>
+        </is>
+      </c>
       <c r="K6" s="241" t="n"/>
-      <c r="L6" s="208" t="n"/>
+      <c r="L6" s="208" t="inlineStr">
+        <is>
+          <t>TECH_PLAS</t>
+        </is>
+      </c>
       <c r="M6" s="241" t="n"/>
-      <c r="N6" s="208" t="n"/>
+      <c r="N6" s="208" t="inlineStr">
+        <is>
+          <t>TECH_PLAS</t>
+        </is>
+      </c>
       <c r="O6" s="241" t="n"/>
       <c r="P6" s="208" t="n"/>
       <c r="Q6" s="241" t="n"/>
@@ -3088,7 +3124,7 @@
       <c r="X6" s="208" t="n"/>
       <c r="Y6" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="7">
+    <row r="7" outlineLevel="1" ht="15" customHeight="1">
       <c r="A7" s="242" t="inlineStr">
         <is>
           <t>Average quantity / a</t>
@@ -3100,13 +3136,21 @@
       <c r="E7" s="241" t="n"/>
       <c r="F7" s="206" t="n"/>
       <c r="G7" s="241" t="n"/>
-      <c r="H7" s="206" t="n"/>
+      <c r="H7" s="206" t="n">
+        <v>434166</v>
+      </c>
       <c r="I7" s="241" t="n"/>
-      <c r="J7" s="206" t="n"/>
+      <c r="J7" s="206" t="n">
+        <v>412000</v>
+      </c>
       <c r="K7" s="241" t="n"/>
-      <c r="L7" s="206" t="n"/>
+      <c r="L7" s="206" t="n">
+        <v>500696</v>
+      </c>
       <c r="M7" s="241" t="n"/>
-      <c r="N7" s="206" t="n"/>
+      <c r="N7" s="206" t="n">
+        <v>500696</v>
+      </c>
       <c r="O7" s="241" t="n"/>
       <c r="P7" s="206" t="n"/>
       <c r="Q7" s="241" t="n"/>
@@ -3119,7 +3163,7 @@
       <c r="X7" s="206" t="n"/>
       <c r="Y7" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="8">
+    <row r="8" outlineLevel="1" ht="15" customHeight="1">
       <c r="A8" s="242" t="inlineStr">
         <is>
           <t>Target cost [€/100 pcs.]</t>
@@ -3131,13 +3175,21 @@
       <c r="E8" s="241" t="n"/>
       <c r="F8" s="204" t="n"/>
       <c r="G8" s="241" t="n"/>
-      <c r="H8" s="204" t="n"/>
+      <c r="H8" s="204" t="n">
+        <v>46.19164619164619</v>
+      </c>
       <c r="I8" s="241" t="n"/>
-      <c r="J8" s="204" t="n"/>
+      <c r="J8" s="204" t="n">
+        <v>62.65356265356265</v>
+      </c>
       <c r="K8" s="241" t="n"/>
-      <c r="L8" s="204" t="n"/>
+      <c r="L8" s="204" t="n">
+        <v>36.85503685503685</v>
+      </c>
       <c r="M8" s="241" t="n"/>
-      <c r="N8" s="204" t="n"/>
+      <c r="N8" s="204" t="n">
+        <v>36.85503685503685</v>
+      </c>
       <c r="O8" s="241" t="n"/>
       <c r="P8" s="204" t="n"/>
       <c r="Q8" s="241" t="n"/>
@@ -3150,7 +3202,7 @@
       <c r="X8" s="204" t="n"/>
       <c r="Y8" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="9">
+    <row r="9" outlineLevel="1" ht="15" customHeight="1">
       <c r="A9" s="242" t="inlineStr">
         <is>
           <t>Project life time [years]</t>
@@ -3161,18 +3213,24 @@
       <c r="D9" s="239" t="n"/>
       <c r="E9" s="241" t="n"/>
       <c r="F9" s="108" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G9" s="241" t="n"/>
       <c r="H9" s="108" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I9" s="241" t="n"/>
-      <c r="J9" s="108" t="n"/>
+      <c r="J9" s="108" t="n">
+        <v>9</v>
+      </c>
       <c r="K9" s="241" t="n"/>
-      <c r="L9" s="108" t="n"/>
+      <c r="L9" s="108" t="n">
+        <v>9</v>
+      </c>
       <c r="M9" s="241" t="n"/>
-      <c r="N9" s="108" t="n"/>
+      <c r="N9" s="108" t="n">
+        <v>9</v>
+      </c>
       <c r="O9" s="241" t="n"/>
       <c r="P9" s="108" t="n"/>
       <c r="Q9" s="241" t="n"/>
@@ -3185,7 +3243,7 @@
       <c r="X9" s="108" t="n"/>
       <c r="Y9" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="10">
+    <row r="10" outlineLevel="1" ht="15" customHeight="1">
       <c r="A10" s="242" t="inlineStr">
         <is>
           <t>Production plant Hella</t>
@@ -3203,11 +3261,17 @@
         <v>1111</v>
       </c>
       <c r="I10" s="241" t="n"/>
-      <c r="J10" s="108" t="n"/>
+      <c r="J10" s="108" t="n">
+        <v>1111</v>
+      </c>
       <c r="K10" s="241" t="n"/>
-      <c r="L10" s="108" t="n"/>
+      <c r="L10" s="108" t="n">
+        <v>1111</v>
+      </c>
       <c r="M10" s="241" t="n"/>
-      <c r="N10" s="108" t="n"/>
+      <c r="N10" s="108" t="n">
+        <v>1111</v>
+      </c>
       <c r="O10" s="241" t="n"/>
       <c r="P10" s="108" t="n"/>
       <c r="Q10" s="241" t="n"/>
@@ -3220,7 +3284,7 @@
       <c r="X10" s="108" t="n"/>
       <c r="Y10" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="12.75" outlineLevel="1" r="11">
+    <row r="11" outlineLevel="1" ht="12.75" customHeight="1">
       <c r="A11" s="242" t="inlineStr">
         <is>
           <t>C- samples [mm.yyyy]</t>
@@ -3238,15 +3302,27 @@
       <c r="G11" s="241" t="n"/>
       <c r="H11" s="110" t="inlineStr">
         <is>
+          <t>08.2019</t>
+        </is>
+      </c>
+      <c r="I11" s="241" t="n"/>
+      <c r="J11" s="110" t="inlineStr">
+        <is>
           <t>in.Unde</t>
         </is>
       </c>
-      <c r="I11" s="241" t="n"/>
-      <c r="J11" s="110" t="n"/>
       <c r="K11" s="241" t="n"/>
-      <c r="L11" s="110" t="n"/>
+      <c r="L11" s="110" t="inlineStr">
+        <is>
+          <t>in.Unde</t>
+        </is>
+      </c>
       <c r="M11" s="241" t="n"/>
-      <c r="N11" s="110" t="n"/>
+      <c r="N11" s="110" t="inlineStr">
+        <is>
+          <t>08.2019</t>
+        </is>
+      </c>
       <c r="O11" s="241" t="n"/>
       <c r="P11" s="110" t="n"/>
       <c r="Q11" s="241" t="n"/>
@@ -3259,7 +3335,7 @@
       <c r="X11" s="110" t="n"/>
       <c r="Y11" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="12">
+    <row r="12" outlineLevel="1" ht="15" customHeight="1">
       <c r="A12" s="242" t="inlineStr">
         <is>
           <t>SOP Hella [mm.yyyy]</t>
@@ -3271,21 +3347,33 @@
       <c r="E12" s="241" t="n"/>
       <c r="F12" s="108" t="inlineStr">
         <is>
-          <t>08.2019</t>
+          <t>10.2020</t>
         </is>
       </c>
       <c r="G12" s="241" t="n"/>
       <c r="H12" s="108" t="inlineStr">
         <is>
-          <t>08.2019</t>
+          <t>10.2020</t>
         </is>
       </c>
       <c r="I12" s="241" t="n"/>
-      <c r="J12" s="108" t="n"/>
+      <c r="J12" s="108" t="inlineStr">
+        <is>
+          <t>10.2020</t>
+        </is>
+      </c>
       <c r="K12" s="241" t="n"/>
-      <c r="L12" s="108" t="n"/>
+      <c r="L12" s="108" t="inlineStr">
+        <is>
+          <t>10.2020</t>
+        </is>
+      </c>
       <c r="M12" s="241" t="n"/>
-      <c r="N12" s="108" t="n"/>
+      <c r="N12" s="108" t="inlineStr">
+        <is>
+          <t>10.2020</t>
+        </is>
+      </c>
       <c r="O12" s="241" t="n"/>
       <c r="P12" s="108" t="n"/>
       <c r="Q12" s="241" t="n"/>
@@ -3298,7 +3386,7 @@
       <c r="X12" s="108" t="n"/>
       <c r="Y12" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="13">
+    <row r="13" outlineLevel="1" ht="15" customHeight="1">
       <c r="A13" s="242" t="inlineStr">
         <is>
           <t>Raw material (acc. to current drawing version)</t>
@@ -3310,21 +3398,33 @@
       <c r="E13" s="241" t="n"/>
       <c r="F13" s="108" t="inlineStr">
         <is>
-          <t>PA6 GF50</t>
+          <t>BEKAERT</t>
         </is>
       </c>
       <c r="G13" s="241" t="n"/>
       <c r="H13" s="108" t="inlineStr">
         <is>
-          <t>PA6 GF50</t>
+          <t>PA66 GF40</t>
         </is>
       </c>
       <c r="I13" s="241" t="n"/>
-      <c r="J13" s="108" t="n"/>
+      <c r="J13" s="108" t="inlineStr">
+        <is>
+          <t>PA66 GF40</t>
+        </is>
+      </c>
       <c r="K13" s="241" t="n"/>
-      <c r="L13" s="108" t="n"/>
+      <c r="L13" s="108" t="inlineStr">
+        <is>
+          <t>PA66 GF40</t>
+        </is>
+      </c>
       <c r="M13" s="241" t="n"/>
-      <c r="N13" s="108" t="n"/>
+      <c r="N13" s="108" t="inlineStr">
+        <is>
+          <t>PA66 GF40</t>
+        </is>
+      </c>
       <c r="O13" s="241" t="n"/>
       <c r="P13" s="108" t="n"/>
       <c r="Q13" s="241" t="n"/>
@@ -3337,7 +3437,7 @@
       <c r="X13" s="108" t="n"/>
       <c r="Y13" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="14">
+    <row r="14" outlineLevel="1" ht="15" customHeight="1">
       <c r="A14" s="242" t="inlineStr">
         <is>
           <t>MGM (Purchasing)</t>
@@ -3359,11 +3459,23 @@
         </is>
       </c>
       <c r="I14" s="241" t="n"/>
-      <c r="J14" s="108" t="n"/>
+      <c r="J14" s="108" t="inlineStr">
+        <is>
+          <t>PlzUpdate</t>
+        </is>
+      </c>
       <c r="K14" s="241" t="n"/>
-      <c r="L14" s="108" t="n"/>
+      <c r="L14" s="108" t="inlineStr">
+        <is>
+          <t>PlzUpdate</t>
+        </is>
+      </c>
       <c r="M14" s="241" t="n"/>
-      <c r="N14" s="108" t="n"/>
+      <c r="N14" s="108" t="inlineStr">
+        <is>
+          <t>PlzUpdate</t>
+        </is>
+      </c>
       <c r="O14" s="241" t="n"/>
       <c r="P14" s="108" t="n"/>
       <c r="Q14" s="241" t="n"/>
@@ -3376,7 +3488,7 @@
       <c r="X14" s="108" t="n"/>
       <c r="Y14" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="15">
+    <row r="15" outlineLevel="1" ht="15" customHeight="1">
       <c r="A15" s="242" t="inlineStr">
         <is>
           <t>Series Purchasing (MGS)</t>
@@ -3388,7 +3500,7 @@
       <c r="E15" s="241" t="n"/>
       <c r="F15" s="110" t="inlineStr">
         <is>
-          <t>Jerry Fang</t>
+          <t>PlzUpdate</t>
         </is>
       </c>
       <c r="G15" s="241" t="n"/>
@@ -3398,11 +3510,23 @@
         </is>
       </c>
       <c r="I15" s="241" t="n"/>
-      <c r="J15" s="110" t="n"/>
+      <c r="J15" s="110" t="inlineStr">
+        <is>
+          <t>Jerry Fang</t>
+        </is>
+      </c>
       <c r="K15" s="241" t="n"/>
-      <c r="L15" s="110" t="n"/>
+      <c r="L15" s="110" t="inlineStr">
+        <is>
+          <t>Jerry Fang</t>
+        </is>
+      </c>
       <c r="M15" s="241" t="n"/>
-      <c r="N15" s="110" t="n"/>
+      <c r="N15" s="110" t="inlineStr">
+        <is>
+          <t>Jerry Fang</t>
+        </is>
+      </c>
       <c r="O15" s="241" t="n"/>
       <c r="P15" s="110" t="n"/>
       <c r="Q15" s="241" t="n"/>
@@ -3415,7 +3539,7 @@
       <c r="X15" s="110" t="n"/>
       <c r="Y15" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="15" outlineLevel="1" r="16">
+    <row r="16" outlineLevel="1" ht="15" customHeight="1">
       <c r="A16" s="242" t="inlineStr">
         <is>
           <t>Project Purchasing</t>
@@ -3437,11 +3561,23 @@
         </is>
       </c>
       <c r="I16" s="241" t="n"/>
-      <c r="J16" s="108" t="n"/>
+      <c r="J16" s="108" t="inlineStr">
+        <is>
+          <t>CHENMI20</t>
+        </is>
+      </c>
       <c r="K16" s="241" t="n"/>
-      <c r="L16" s="108" t="n"/>
+      <c r="L16" s="108" t="inlineStr">
+        <is>
+          <t>CHENMI20</t>
+        </is>
+      </c>
       <c r="M16" s="241" t="n"/>
-      <c r="N16" s="108" t="n"/>
+      <c r="N16" s="108" t="inlineStr">
+        <is>
+          <t>CHENMI20</t>
+        </is>
+      </c>
       <c r="O16" s="241" t="n"/>
       <c r="P16" s="108" t="n"/>
       <c r="Q16" s="241" t="n"/>
@@ -3454,7 +3590,7 @@
       <c r="X16" s="108" t="n"/>
       <c r="Y16" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="12.75" outlineLevel="1" r="17">
+    <row r="17" outlineLevel="1" ht="12.75" customHeight="1">
       <c r="A17" s="242" t="inlineStr">
         <is>
           <t>General comment</t>
@@ -3485,7 +3621,7 @@
       <c r="X17" s="108" t="n"/>
       <c r="Y17" s="243" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" outlineLevel="1" r="18" thickBot="1">
+    <row r="18" outlineLevel="1" ht="13.5" customHeight="1" thickBot="1">
       <c r="A18" s="244" t="n"/>
       <c r="B18" s="233" t="n"/>
       <c r="C18" s="233" t="n"/>
@@ -3512,7 +3648,7 @@
       <c r="X18" s="244" t="n"/>
       <c r="Y18" s="245" t="n"/>
     </row>
-    <row customHeight="1" ht="17.25" r="19" thickBot="1">
+    <row r="19" ht="17.25" customHeight="1" thickBot="1">
       <c r="A19" s="12" t="n"/>
       <c r="B19" s="11" t="n"/>
       <c r="C19" s="11" t="n"/>
@@ -3539,7 +3675,7 @@
       <c r="X19" s="8" t="n"/>
       <c r="Y19" s="10" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="20" thickBot="1">
+    <row r="20" ht="15.75" customHeight="1" thickBot="1">
       <c r="A20" s="34" t="n"/>
       <c r="B20" s="7" t="n"/>
       <c r="C20" s="7" t="n"/>
@@ -3606,7 +3742,7 @@
       </c>
       <c r="Y20" s="246" t="n"/>
     </row>
-    <row customHeight="1" ht="97.5" r="21" thickBot="1">
+    <row r="21" ht="97.5" customHeight="1" thickBot="1">
       <c r="A21" s="37" t="inlineStr">
         <is>
           <t>I</t>
@@ -3690,7 +3826,7 @@
       </c>
       <c r="Y21" s="246" t="n"/>
     </row>
-    <row customHeight="1" ht="17.25" outlineLevel="1" r="22" thickBot="1">
+    <row r="22" outlineLevel="1" ht="17.25" customHeight="1" thickBot="1">
       <c r="A22" s="60" t="n"/>
       <c r="B22" s="61" t="inlineStr">
         <is>
@@ -3809,7 +3945,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="63.75" outlineLevel="1" r="23">
+    <row r="23" outlineLevel="1" ht="63.75" customHeight="1">
       <c r="A23" s="113" t="n">
         <v>1</v>
       </c>
@@ -3877,7 +4013,7 @@
       </c>
       <c r="Y23" s="19" t="n"/>
     </row>
-    <row customHeight="1" ht="63.75" outlineLevel="1" r="24">
+    <row r="24" outlineLevel="1" ht="63.75" customHeight="1">
       <c r="A24" s="248" t="n"/>
       <c r="B24" s="249" t="n"/>
       <c r="C24" s="145" t="inlineStr">
@@ -3939,7 +4075,7 @@
       </c>
       <c r="Y24" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="114.75" outlineLevel="1" r="25">
+    <row r="25" outlineLevel="1" ht="114.75" customHeight="1">
       <c r="A25" s="248" t="n"/>
       <c r="B25" s="249" t="n"/>
       <c r="C25" s="145" t="inlineStr">
@@ -4001,7 +4137,7 @@
       </c>
       <c r="Y25" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="89.25" outlineLevel="1" r="26">
+    <row r="26" outlineLevel="1" ht="89.25" customHeight="1">
       <c r="A26" s="248" t="n"/>
       <c r="B26" s="249" t="n"/>
       <c r="C26" s="145" t="inlineStr">
@@ -4064,7 +4200,7 @@
       </c>
       <c r="Y26" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="192" outlineLevel="1" r="27" thickBot="1">
+    <row r="27" outlineLevel="1" ht="192" customHeight="1" thickBot="1">
       <c r="A27" s="250" t="n"/>
       <c r="B27" s="235" t="n"/>
       <c r="C27" s="64" t="inlineStr">
@@ -4108,7 +4244,7 @@
       <c r="X27" s="20" t="n"/>
       <c r="Y27" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="51" outlineLevel="1" r="28">
+    <row r="28" outlineLevel="1" ht="51" customHeight="1">
       <c r="A28" s="163" t="n">
         <v>2</v>
       </c>
@@ -4179,7 +4315,7 @@
       </c>
       <c r="Y28" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="51" outlineLevel="1" r="29">
+    <row r="29" outlineLevel="1" ht="51" customHeight="1">
       <c r="A29" s="248" t="n"/>
       <c r="B29" s="249" t="n"/>
       <c r="C29" s="235" t="n"/>
@@ -4233,7 +4369,7 @@
       </c>
       <c r="Y29" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="102" outlineLevel="1" r="30">
+    <row r="30" outlineLevel="1" ht="102" customHeight="1">
       <c r="A30" s="248" t="n"/>
       <c r="B30" s="249" t="n"/>
       <c r="C30" s="145" t="inlineStr">
@@ -4295,7 +4431,7 @@
       </c>
       <c r="Y30" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="90" outlineLevel="1" r="31" thickBot="1">
+    <row r="31" outlineLevel="1" ht="90" customHeight="1" thickBot="1">
       <c r="A31" s="250" t="n"/>
       <c r="B31" s="235" t="n"/>
       <c r="C31" s="64" t="inlineStr">
@@ -4358,7 +4494,7 @@
       </c>
       <c r="Y31" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="102" outlineLevel="1" r="32">
+    <row r="32" outlineLevel="1" ht="102" customHeight="1">
       <c r="A32" s="163" t="n">
         <v>3</v>
       </c>
@@ -4427,7 +4563,7 @@
       </c>
       <c r="Y32" s="19" t="n"/>
     </row>
-    <row customHeight="1" ht="76.5" outlineLevel="1" r="33">
+    <row r="33" outlineLevel="1" ht="76.5" customHeight="1">
       <c r="A33" s="248" t="n"/>
       <c r="B33" s="249" t="n"/>
       <c r="C33" s="145" t="inlineStr">
@@ -4488,7 +4624,7 @@
       </c>
       <c r="Y33" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="89.25" outlineLevel="1" r="34">
+    <row r="34" outlineLevel="1" ht="89.25" customHeight="1">
       <c r="A34" s="248" t="n"/>
       <c r="B34" s="249" t="n"/>
       <c r="C34" s="145" t="inlineStr">
@@ -4550,7 +4686,7 @@
       </c>
       <c r="Y34" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="35" thickBot="1">
+    <row r="35" outlineLevel="1" ht="39" customHeight="1" thickBot="1">
       <c r="A35" s="250" t="n"/>
       <c r="B35" s="235" t="n"/>
       <c r="C35" s="64" t="inlineStr">
@@ -4611,7 +4747,7 @@
       </c>
       <c r="Y35" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="127.5" outlineLevel="1" r="36">
+    <row r="36" outlineLevel="1" ht="127.5" customHeight="1">
       <c r="A36" s="163" t="n">
         <v>4</v>
       </c>
@@ -4679,7 +4815,7 @@
       </c>
       <c r="Y36" s="19" t="n"/>
     </row>
-    <row customHeight="1" ht="114.75" outlineLevel="1" r="37">
+    <row r="37" outlineLevel="1" ht="114.75" customHeight="1">
       <c r="A37" s="248" t="n"/>
       <c r="B37" s="249" t="n"/>
       <c r="C37" s="145" t="inlineStr">
@@ -4741,7 +4877,7 @@
       </c>
       <c r="Y37" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="102.75" outlineLevel="1" r="38" thickBot="1">
+    <row r="38" outlineLevel="1" ht="102.75" customHeight="1" thickBot="1">
       <c r="A38" s="250" t="n"/>
       <c r="B38" s="235" t="n"/>
       <c r="C38" s="64" t="inlineStr">
@@ -4804,7 +4940,7 @@
       </c>
       <c r="Y38" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="30" outlineLevel="1" r="39">
+    <row r="39" outlineLevel="1" ht="30" customHeight="1">
       <c r="A39" s="163" t="n">
         <v>5</v>
       </c>
@@ -4871,7 +5007,7 @@
       </c>
       <c r="Y39" s="19" t="n"/>
     </row>
-    <row customHeight="1" ht="30" outlineLevel="1" r="40" thickBot="1">
+    <row r="40" outlineLevel="1" ht="30" customHeight="1" thickBot="1">
       <c r="A40" s="250" t="n"/>
       <c r="B40" s="235" t="n"/>
       <c r="C40" s="56" t="inlineStr">
@@ -4930,7 +5066,7 @@
       </c>
       <c r="Y40" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" outlineLevel="1" r="41" thickBot="1">
+    <row r="41" outlineLevel="1" ht="13.5" customHeight="1" thickBot="1">
       <c r="A41" s="34" t="n"/>
       <c r="B41" s="35" t="inlineStr">
         <is>
@@ -4961,7 +5097,7 @@
       <c r="X41" s="27" t="n"/>
       <c r="Y41" s="27" t="n"/>
     </row>
-    <row customHeight="1" ht="22.5" outlineLevel="1" r="42" thickBot="1">
+    <row r="42" outlineLevel="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A42" s="34" t="n"/>
       <c r="B42" s="5" t="inlineStr">
         <is>
@@ -5030,7 +5166,7 @@
       </c>
       <c r="Y42" s="246" t="n"/>
     </row>
-    <row customHeight="1" ht="22.5" outlineLevel="1" r="43" thickBot="1">
+    <row r="43" outlineLevel="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A43" s="34" t="n"/>
       <c r="B43" s="5" t="inlineStr">
         <is>
@@ -5099,7 +5235,7 @@
       </c>
       <c r="Y43" s="246" t="n"/>
     </row>
-    <row customHeight="1" ht="22.5" outlineLevel="1" r="44" thickBot="1">
+    <row r="44" outlineLevel="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A44" s="34" t="n"/>
       <c r="B44" s="36" t="inlineStr">
         <is>
@@ -5136,7 +5272,7 @@
       <c r="X44" s="194" t="n"/>
       <c r="Y44" s="246" t="n"/>
     </row>
-    <row customHeight="1" ht="16.5" r="45" thickBot="1">
+    <row r="45" ht="16.5" customHeight="1" thickBot="1">
       <c r="A45" s="37" t="inlineStr">
         <is>
           <t>II</t>
@@ -5171,7 +5307,7 @@
       <c r="X45" s="29" t="n"/>
       <c r="Y45" s="29" t="n"/>
     </row>
-    <row customHeight="1" ht="20.25" r="46" thickBot="1">
+    <row r="46" ht="20.25" customHeight="1" thickBot="1">
       <c r="A46" s="39" t="n"/>
       <c r="B46" s="195" t="inlineStr">
         <is>
@@ -5246,7 +5382,7 @@
       </c>
       <c r="Y46" s="246" t="n"/>
     </row>
-    <row customHeight="1" ht="32.25" r="47">
+    <row r="47" ht="32.25" customHeight="1">
       <c r="A47" s="166" t="n">
         <v>1</v>
       </c>
@@ -5328,7 +5464,7 @@
       </c>
       <c r="Y47" s="238" t="n"/>
     </row>
-    <row customHeight="1" ht="32.25" r="48">
+    <row r="48" ht="32.25" customHeight="1">
       <c r="A48" s="248" t="n"/>
       <c r="B48" s="249" t="n"/>
       <c r="C48" s="145" t="inlineStr">
@@ -5403,7 +5539,7 @@
       </c>
       <c r="Y48" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="32.25" r="49">
+    <row r="49" ht="32.25" customHeight="1">
       <c r="A49" s="248" t="n"/>
       <c r="B49" s="249" t="n"/>
       <c r="C49" s="145" t="inlineStr">
@@ -5478,7 +5614,7 @@
       </c>
       <c r="Y49" s="241" t="n"/>
     </row>
-    <row customHeight="1" ht="32.25" r="50" thickBot="1">
+    <row r="50" ht="32.25" customHeight="1" thickBot="1">
       <c r="A50" s="250" t="n"/>
       <c r="B50" s="235" t="n"/>
       <c r="C50" s="64" t="inlineStr">
@@ -5553,7 +5689,7 @@
       </c>
       <c r="Y50" s="255" t="n"/>
     </row>
-    <row customHeight="1" ht="17.25" r="51" thickBot="1">
+    <row r="51" ht="17.25" customHeight="1" thickBot="1">
       <c r="A51" s="163" t="n">
         <v>2</v>
       </c>
@@ -5590,7 +5726,7 @@
       <c r="X51" s="17" t="n"/>
       <c r="Y51" s="17" t="n"/>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="52">
+    <row r="52" outlineLevel="1" ht="39" customHeight="1">
       <c r="A52" s="248" t="n"/>
       <c r="B52" s="249" t="n"/>
       <c r="C52" s="145" t="inlineStr">
@@ -5705,7 +5841,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="53">
+    <row r="53" outlineLevel="1" ht="39" customHeight="1">
       <c r="A53" s="248" t="n"/>
       <c r="B53" s="249" t="n"/>
       <c r="C53" s="145" t="inlineStr">
@@ -5820,7 +5956,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="54">
+    <row r="54" outlineLevel="1" ht="39" customHeight="1">
       <c r="A54" s="248" t="n"/>
       <c r="B54" s="249" t="n"/>
       <c r="C54" s="145" t="inlineStr">
@@ -5936,7 +6072,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="55">
+    <row r="55" outlineLevel="1" ht="39" customHeight="1">
       <c r="A55" s="248" t="n"/>
       <c r="B55" s="249" t="n"/>
       <c r="C55" s="145" t="inlineStr">
@@ -6051,7 +6187,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="56">
+    <row r="56" outlineLevel="1" ht="39" customHeight="1">
       <c r="A56" s="248" t="n"/>
       <c r="B56" s="249" t="n"/>
       <c r="C56" s="145" t="inlineStr">
@@ -6166,7 +6302,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="57">
+    <row r="57" outlineLevel="1" ht="39" customHeight="1">
       <c r="A57" s="248" t="n"/>
       <c r="B57" s="249" t="n"/>
       <c r="C57" s="145" t="inlineStr">
@@ -6281,7 +6417,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="39" outlineLevel="1" r="58" thickBot="1">
+    <row r="58" outlineLevel="1" ht="39" customHeight="1" thickBot="1">
       <c r="A58" s="250" t="n"/>
       <c r="B58" s="235" t="n"/>
       <c r="C58" s="56" t="inlineStr">
@@ -6396,7 +6532,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="25.5" r="59" thickBot="1">
+    <row r="59" ht="25.5" customHeight="1" thickBot="1">
       <c r="A59" s="41" t="n"/>
       <c r="B59" s="7" t="n"/>
       <c r="C59" s="7" t="n"/>
@@ -6423,7 +6559,7 @@
       <c r="X59" s="7" t="n"/>
       <c r="Y59" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="16.5" r="60" thickBot="1">
+    <row r="60" ht="16.5" customHeight="1" thickBot="1">
       <c r="A60" s="82" t="inlineStr">
         <is>
           <t>III</t>
@@ -6458,7 +6594,7 @@
       <c r="X60" s="259" t="n"/>
       <c r="Y60" s="251" t="n"/>
     </row>
-    <row customHeight="1" ht="25.5" r="61" thickBot="1">
+    <row r="61" ht="25.5" customHeight="1" thickBot="1">
       <c r="A61" s="84" t="n">
         <v>1</v>
       </c>
@@ -6527,7 +6663,7 @@
       </c>
       <c r="Y61" s="263" t="n"/>
     </row>
-    <row customHeight="1" ht="25.5" r="62">
+    <row r="62" ht="25.5" customHeight="1">
       <c r="A62" s="166" t="n">
         <v>2</v>
       </c>
@@ -6596,7 +6732,7 @@
       </c>
       <c r="Y62" s="261" t="n"/>
     </row>
-    <row customHeight="1" ht="25.5" r="63">
+    <row r="63" ht="25.5" customHeight="1">
       <c r="A63" s="248" t="n"/>
       <c r="B63" s="249" t="n"/>
       <c r="C63" s="88" t="n">
@@ -6659,7 +6795,7 @@
       </c>
       <c r="Y63" s="254" t="n"/>
     </row>
-    <row customHeight="1" ht="25.5" r="64" thickBot="1">
+    <row r="64" ht="25.5" customHeight="1" thickBot="1">
       <c r="A64" s="250" t="n"/>
       <c r="B64" s="235" t="n"/>
       <c r="C64" s="89" t="n">
@@ -6722,7 +6858,7 @@
       </c>
       <c r="Y64" s="257" t="n"/>
     </row>
-    <row customHeight="1" ht="27" r="65" thickBot="1">
+    <row r="65" ht="27" customHeight="1" thickBot="1">
       <c r="A65" s="83" t="n">
         <v>3</v>
       </c>
@@ -7162,51 +7298,51 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="F65:Y65">
-    <cfRule dxfId="3" operator="equal" priority="10" type="cellIs">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="3">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V65:Y65">
-    <cfRule dxfId="3" operator="equal" priority="9" type="cellIs">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="3">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61:Y61 F43:Y43 F65:Y65">
-    <cfRule dxfId="2" operator="equal" priority="11" type="cellIs">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="2">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule dxfId="1" operator="equal" priority="12" type="cellIs">
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="1">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="equal" priority="13" type="cellIs">
+    <cfRule type="cellIs" priority="13" operator="equal" dxfId="0">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7" disablePrompts="1">
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="X52 V52 T52 R52 P52 N52 L52 J52 H52 F52" type="list">
+  <dataValidations disablePrompts="1" count="7">
+    <dataValidation sqref="X52 V52 T52 R52 P52 N52 L52 J52 H52 F52" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"&gt;&gt;Please select,Single Sourcing,2nd Source,Multiple Sourcing"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="X56 V56 T56 R56 P56 N56 L56 J56 H56 F56" type="list">
+    <dataValidation sqref="X56 V56 T56 R56 P56 N56 L56 J56 H56 F56" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"&gt;&gt;Please select,with other projects,with other customer demands,with other production locations,not relevant"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="F54 H54 J54 L54 N54 P54 R54 T54 V54 X54" type="list">
+    <dataValidation sqref="F54 H54 J54 L54 N54 P54 R54 T54 V54 X54" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"&gt;&gt;Please select,Low,Medium,High"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="F53 H53 J53 L53 N53 P53 R53 T53 V53 X53" type="list">
+    <dataValidation sqref="F53 H53 J53 L53 N53 P53 R53 T53 V53 X53" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"&gt;&gt;Please select,Best Cost,based on customer requirements,to be further discussed,not relevant"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="W52:W58 G52:G58 I52:I58 K52:K58 M52:M58 O52:O58 Q52:Q58 S52:S58 U52:U58 Y52:Y58" type="list">
+    <dataValidation sqref="W52:W58 G52:G58 I52:I58 K52:K58 M52:M58 O52:O58 Q52:Q58 S52:S58 U52:U58 Y52:Y58" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"&gt;&gt; Please rank,1,2,3,4,5,6,7"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="F55 H55 J55 L55 N55 P55 R55 T55 V55 X55 F57 H57 J57 L57 N57 P57 R57 T57 V57 X57" type="list">
+    <dataValidation sqref="F55 H55 J55 L55 N55 P55 R55 T55 V55 X55 F57 H57 J57 L57 N57 P57 R57 T57 V57 X57" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"&gt;&gt; Please select,yes,no"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="X23:X40 V23:V40 T23:T40 R23:R40 P23:P40 N23:N40 L23:L40 J23:J40 H23:H40 F23:F40" type="list">
+    <dataValidation sqref="X23:X40 V23:V40 T23:T40 R23:R40 P23:P40 N23:N40 L23:L40 J23:J40 H23:H40 F23:F40" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.5905511811023623" footer="0.3149606299212598" header="0.3149606299212598" left="0.3149606299212598" right="0.3149606299212598" top="0.3937007874015748"/>
-  <pageSetup fitToHeight="0" orientation="portrait" paperSize="9" scale="80"/>
+  <pageMargins left="0.3149606299212598" right="0.3149606299212598" top="0.3937007874015748" bottom="0.5905511811023623" header="0.3149606299212598" footer="0.3149606299212598"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="80" fitToHeight="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor re injectioin function done
</commit_message>
<xml_diff>
--- a/output/risk_eval_output.xlsx
+++ b/output/risk_eval_output.xlsx
@@ -3005,11 +3005,7 @@
         </is>
       </c>
       <c r="M4" s="241" t="n"/>
-      <c r="N4" s="213" t="inlineStr">
-        <is>
-          <t>323.140-00</t>
-        </is>
-      </c>
+      <c r="N4" s="213" t="n"/>
       <c r="O4" s="241" t="n"/>
       <c r="P4" s="212" t="n"/>
       <c r="Q4" s="241" t="n"/>
@@ -3056,11 +3052,7 @@
         </is>
       </c>
       <c r="M5" s="241" t="n"/>
-      <c r="N5" s="136" t="inlineStr">
-        <is>
-          <t>GEHAEUSE MONT-GR</t>
-        </is>
-      </c>
+      <c r="N5" s="136" t="n"/>
       <c r="O5" s="241" t="n"/>
       <c r="P5" s="136" t="n"/>
       <c r="Q5" s="241" t="n"/>
@@ -3107,11 +3099,7 @@
         </is>
       </c>
       <c r="M6" s="241" t="n"/>
-      <c r="N6" s="208" t="inlineStr">
-        <is>
-          <t>TECH_PLAS</t>
-        </is>
-      </c>
+      <c r="N6" s="208" t="n"/>
       <c r="O6" s="241" t="n"/>
       <c r="P6" s="208" t="n"/>
       <c r="Q6" s="241" t="n"/>
@@ -3148,9 +3136,7 @@
         <v>500696</v>
       </c>
       <c r="M7" s="241" t="n"/>
-      <c r="N7" s="206" t="n">
-        <v>500696</v>
-      </c>
+      <c r="N7" s="206" t="n"/>
       <c r="O7" s="241" t="n"/>
       <c r="P7" s="206" t="n"/>
       <c r="Q7" s="241" t="n"/>
@@ -3176,20 +3162,18 @@
       <c r="F8" s="204" t="n"/>
       <c r="G8" s="241" t="n"/>
       <c r="H8" s="204" t="n">
-        <v>46.19164619164619</v>
+        <v>4.705436171336311</v>
       </c>
       <c r="I8" s="241" t="n"/>
       <c r="J8" s="204" t="n">
-        <v>62.65356265356265</v>
+        <v>6.961506961506961</v>
       </c>
       <c r="K8" s="241" t="n"/>
       <c r="L8" s="204" t="n">
-        <v>36.85503685503685</v>
+        <v>4.095004095004094</v>
       </c>
       <c r="M8" s="241" t="n"/>
-      <c r="N8" s="204" t="n">
-        <v>36.85503685503685</v>
-      </c>
+      <c r="N8" s="204" t="n"/>
       <c r="O8" s="241" t="n"/>
       <c r="P8" s="204" t="n"/>
       <c r="Q8" s="241" t="n"/>
@@ -3213,7 +3197,7 @@
       <c r="D9" s="239" t="n"/>
       <c r="E9" s="241" t="n"/>
       <c r="F9" s="108" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G9" s="241" t="n"/>
       <c r="H9" s="108" t="n">
@@ -3228,9 +3212,7 @@
         <v>9</v>
       </c>
       <c r="M9" s="241" t="n"/>
-      <c r="N9" s="108" t="n">
-        <v>9</v>
-      </c>
+      <c r="N9" s="108" t="n"/>
       <c r="O9" s="241" t="n"/>
       <c r="P9" s="108" t="n"/>
       <c r="Q9" s="241" t="n"/>
@@ -3269,9 +3251,7 @@
         <v>1111</v>
       </c>
       <c r="M10" s="241" t="n"/>
-      <c r="N10" s="108" t="n">
-        <v>1111</v>
-      </c>
+      <c r="N10" s="108" t="n"/>
       <c r="O10" s="241" t="n"/>
       <c r="P10" s="108" t="n"/>
       <c r="Q10" s="241" t="n"/>
@@ -3294,11 +3274,7 @@
       <c r="C11" s="239" t="n"/>
       <c r="D11" s="239" t="n"/>
       <c r="E11" s="241" t="n"/>
-      <c r="F11" s="110" t="inlineStr">
-        <is>
-          <t>in.Unde</t>
-        </is>
-      </c>
+      <c r="F11" s="110" t="n"/>
       <c r="G11" s="241" t="n"/>
       <c r="H11" s="110" t="inlineStr">
         <is>
@@ -3306,23 +3282,11 @@
         </is>
       </c>
       <c r="I11" s="241" t="n"/>
-      <c r="J11" s="110" t="inlineStr">
-        <is>
-          <t>in.Unde</t>
-        </is>
-      </c>
+      <c r="J11" s="110" t="n"/>
       <c r="K11" s="241" t="n"/>
-      <c r="L11" s="110" t="inlineStr">
-        <is>
-          <t>in.Unde</t>
-        </is>
-      </c>
+      <c r="L11" s="110" t="n"/>
       <c r="M11" s="241" t="n"/>
-      <c r="N11" s="110" t="inlineStr">
-        <is>
-          <t>08.2019</t>
-        </is>
-      </c>
+      <c r="N11" s="110" t="n"/>
       <c r="O11" s="241" t="n"/>
       <c r="P11" s="110" t="n"/>
       <c r="Q11" s="241" t="n"/>
@@ -3345,35 +3309,19 @@
       <c r="C12" s="239" t="n"/>
       <c r="D12" s="239" t="n"/>
       <c r="E12" s="241" t="n"/>
-      <c r="F12" s="108" t="inlineStr">
-        <is>
-          <t>10.2020</t>
-        </is>
-      </c>
+      <c r="F12" s="108" t="n"/>
       <c r="G12" s="241" t="n"/>
       <c r="H12" s="108" t="inlineStr">
         <is>
-          <t>10.2020</t>
+          <t>9-08-02 00:00:00</t>
         </is>
       </c>
       <c r="I12" s="241" t="n"/>
-      <c r="J12" s="108" t="inlineStr">
-        <is>
-          <t>10.2020</t>
-        </is>
-      </c>
+      <c r="J12" s="108" t="n"/>
       <c r="K12" s="241" t="n"/>
-      <c r="L12" s="108" t="inlineStr">
-        <is>
-          <t>10.2020</t>
-        </is>
-      </c>
+      <c r="L12" s="108" t="n"/>
       <c r="M12" s="241" t="n"/>
-      <c r="N12" s="108" t="inlineStr">
-        <is>
-          <t>10.2020</t>
-        </is>
-      </c>
+      <c r="N12" s="108" t="n"/>
       <c r="O12" s="241" t="n"/>
       <c r="P12" s="108" t="n"/>
       <c r="Q12" s="241" t="n"/>
@@ -3420,11 +3368,7 @@
         </is>
       </c>
       <c r="M13" s="241" t="n"/>
-      <c r="N13" s="108" t="inlineStr">
-        <is>
-          <t>PA66 GF40</t>
-        </is>
-      </c>
+      <c r="N13" s="108" t="n"/>
       <c r="O13" s="241" t="n"/>
       <c r="P13" s="108" t="n"/>
       <c r="Q13" s="241" t="n"/>
@@ -3471,11 +3415,7 @@
         </is>
       </c>
       <c r="M14" s="241" t="n"/>
-      <c r="N14" s="108" t="inlineStr">
-        <is>
-          <t>PlzUpdate</t>
-        </is>
-      </c>
+      <c r="N14" s="108" t="n"/>
       <c r="O14" s="241" t="n"/>
       <c r="P14" s="108" t="n"/>
       <c r="Q14" s="241" t="n"/>
@@ -3522,11 +3462,7 @@
         </is>
       </c>
       <c r="M15" s="241" t="n"/>
-      <c r="N15" s="110" t="inlineStr">
-        <is>
-          <t>Jerry Fang</t>
-        </is>
-      </c>
+      <c r="N15" s="110" t="n"/>
       <c r="O15" s="241" t="n"/>
       <c r="P15" s="110" t="n"/>
       <c r="Q15" s="241" t="n"/>
@@ -3573,11 +3509,7 @@
         </is>
       </c>
       <c r="M16" s="241" t="n"/>
-      <c r="N16" s="108" t="inlineStr">
-        <is>
-          <t>CHENMI20</t>
-        </is>
-      </c>
+      <c r="N16" s="108" t="n"/>
       <c r="O16" s="241" t="n"/>
       <c r="P16" s="108" t="n"/>
       <c r="Q16" s="241" t="n"/>

</xml_diff>